<commit_message>
updated initializeSheet method, update pdf saver, add rebootmeal command
</commit_message>
<xml_diff>
--- a/data/mealdata.xlsx
+++ b/data/mealdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,217 +466,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01-05-2023</t>
+          <t>01-06-2023</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02-05-2023</t>
+          <t>02-06-2023</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03-05-2023</t>
+          <t>03-06-2023</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04-05-2023</t>
+          <t>04-06-2023</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05-05-2023</t>
+          <t>05-06-2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06-05-2023</t>
+          <t>06-06-2023</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>07-05-2023</t>
+          <t>07-06-2023</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>08-05-2023</t>
+          <t>08-06-2023</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>09-05-2023</t>
+          <t>09-06-2023</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10-05-2023</t>
+          <t>10-06-2023</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11-05-2023</t>
+          <t>11-06-2023</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12-05-2023</t>
+          <t>12-06-2023</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13-05-2023</t>
+          <t>13-06-2023</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14-05-2023</t>
+          <t>14-06-2023</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15-05-2023</t>
+          <t>15-06-2023</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16-05-2023</t>
+          <t>16-06-2023</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17-05-2023</t>
+          <t>17-06-2023</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18-05-2023</t>
+          <t>18-06-2023</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19-05-2023</t>
+          <t>19-06-2023</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20-05-2023</t>
+          <t>20-06-2023</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21-05-2023</t>
+          <t>21-06-2023</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22-05-2023</t>
+          <t>22-06-2023</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23-05-2023</t>
+          <t>23-06-2023</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24-05-2023</t>
+          <t>24-06-2023</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25-05-2023</t>
+          <t>25-06-2023</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26-05-2023</t>
+          <t>26-06-2023</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27-05-2023</t>
+          <t>27-06-2023</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28-05-2023</t>
+          <t>28-06-2023</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29-05-2023</t>
+          <t>29-06-2023</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30-05-2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>31-05-2023</t>
+          <t>30-06-2023</t>
         </is>
       </c>
     </row>

</xml_diff>